<commit_message>
posted m2 solutions and updated gradeline spreadsheet
</commit_message>
<xml_diff>
--- a/418_S25/gradelines.xlsx
+++ b/418_S25/gradelines.xlsx
@@ -460,7 +460,7 @@
       </c>
       <c r="D2" s="2">
         <f>100*(SUM(E6:E15)/COUNT(E6:E15)*0.25 + SUM(E20:E22)*0.15 + E23*0.3)</f>
-        <v>22.5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3">
@@ -534,7 +534,7 @@
         <v>20.0</v>
       </c>
       <c r="E9" s="7">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>16</v>
@@ -574,12 +574,14 @@
       </c>
       <c r="H10" s="8">
         <f>0.93*D16</f>
-        <v>55.8</v>
+        <v>74.4</v>
       </c>
       <c r="I10" s="8">
         <v>56.0</v>
       </c>
-      <c r="J10" s="8"/>
+      <c r="J10" s="8">
+        <v>60.0</v>
+      </c>
       <c r="K10" s="7"/>
       <c r="L10" s="8"/>
       <c r="M10" s="8">
@@ -603,17 +605,19 @@
       </c>
       <c r="H11" s="8">
         <f>0.9*D16</f>
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="I11" s="8">
         <v>50.0</v>
       </c>
-      <c r="J11" s="8"/>
+      <c r="J11" s="8">
+        <v>53.0</v>
+      </c>
       <c r="K11" s="7"/>
       <c r="L11" s="8"/>
       <c r="M11" s="8">
         <f>IF(D16=0, 0, H11/D16)*H23 + IF(D20=0, 0, I11/D20)*I23 + IF(D21=0, 0, J11/D21)*J23 + IF(D22=0, 0, K11/D22)*K23 + IF(D23=0, 0, L11/D23)*L23</f>
-        <v>76.07142857</v>
+        <v>75.78571429</v>
       </c>
     </row>
     <row r="12">
@@ -632,17 +636,19 @@
       </c>
       <c r="H12" s="8">
         <f>0.87*D16</f>
-        <v>52.2</v>
+        <v>69.6</v>
       </c>
       <c r="I12" s="8">
         <v>44.0</v>
       </c>
-      <c r="J12" s="8"/>
+      <c r="J12" s="8">
+        <v>46.0</v>
+      </c>
       <c r="K12" s="7"/>
       <c r="L12" s="8"/>
       <c r="M12" s="8">
         <f>IF(D16=0, 0, H12/D16)*H23 + IF(D20=0, 0, I12/D20)*I23 + IF(D21=0, 0, J12/D21)*J23 + IF(D22=0, 0, K12/D22)*K23 + IF(D23=0, 0, L12/D23)*L23</f>
-        <v>68.89285714</v>
+        <v>68.32142857</v>
       </c>
     </row>
     <row r="13">
@@ -661,17 +667,19 @@
       </c>
       <c r="H13" s="8">
         <f>0.83*D16</f>
-        <v>49.8</v>
+        <v>66.4</v>
       </c>
       <c r="I13" s="8">
         <v>38.0</v>
       </c>
-      <c r="J13" s="8"/>
+      <c r="J13" s="8">
+        <v>39.0</v>
+      </c>
       <c r="K13" s="7"/>
       <c r="L13" s="8"/>
       <c r="M13" s="8">
         <f>IF(D16=0, 0, H13/D16)*H23 + IF(D20=0, 0, I13/D20)*I23 + IF(D21=0, 0, J13/D21)*J23 + IF(D22=0, 0, K13/D22)*K23 + IF(D23=0, 0, L13/D23)*L23</f>
-        <v>61.46428571</v>
+        <v>60.60714286</v>
       </c>
     </row>
     <row r="14">
@@ -690,17 +698,19 @@
       </c>
       <c r="H14" s="8">
         <f>0.8*D16</f>
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="I14" s="8">
         <v>32.0</v>
       </c>
-      <c r="J14" s="8"/>
+      <c r="J14" s="8">
+        <v>32.0</v>
+      </c>
       <c r="K14" s="7"/>
       <c r="L14" s="8"/>
       <c r="M14" s="8">
         <f>IF(D16=0, 0, H14/D16)*H23 + IF(D20=0, 0, I14/D20)*I23 + IF(D21=0, 0, J14/D21)*J23 + IF(D22=0, 0, K14/D22)*K23 + IF(D23=0, 0, L14/D23)*L23</f>
-        <v>54.28571429</v>
+        <v>53.14285714</v>
       </c>
     </row>
     <row r="15">
@@ -719,17 +729,19 @@
       </c>
       <c r="H15" s="8">
         <f>0.77*D16</f>
-        <v>46.2</v>
+        <v>61.6</v>
       </c>
       <c r="I15" s="8">
         <v>26.0</v>
       </c>
-      <c r="J15" s="8"/>
+      <c r="J15" s="8">
+        <v>25.0</v>
+      </c>
       <c r="K15" s="7"/>
       <c r="L15" s="8"/>
       <c r="M15" s="8">
         <f>IF(D16=0, 0, H15/D16)*H23 + IF(D20=0, 0, I15/D20)*I23 + IF(D21=0, 0, J15/D21)*J23 + IF(D22=0, 0, K15/D22)*K23 + IF(D23=0, 0, L15/D23)*L23</f>
-        <v>47.10714286</v>
+        <v>45.67857143</v>
       </c>
     </row>
     <row r="16">
@@ -742,7 +754,7 @@
       </c>
       <c r="D16" s="7">
         <f>20*MIN(SUM(E6:E15),COUNT(E6:E15)-1)</f>
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="E16" s="7">
         <v>0.0</v>
@@ -752,17 +764,19 @@
       </c>
       <c r="H16" s="8">
         <f>0.73*D16</f>
-        <v>43.8</v>
+        <v>58.4</v>
       </c>
       <c r="I16" s="8">
         <v>20.0</v>
       </c>
-      <c r="J16" s="8"/>
+      <c r="J16" s="8">
+        <v>20.0</v>
+      </c>
       <c r="K16" s="7"/>
       <c r="L16" s="8"/>
       <c r="M16" s="8">
         <f>IF(D16=0, 0, H16/D16)*H23 + IF(D20=0, 0, I16/D20)*I23 + IF(D21=0, 0, J16/D21)*J23 + IF(D22=0, 0, K16/D22)*K23 + IF(D23=0, 0, L16/D23)*L23</f>
-        <v>39.67857143</v>
+        <v>38.96428571</v>
       </c>
     </row>
     <row r="17">
@@ -771,12 +785,14 @@
       </c>
       <c r="H17" s="8">
         <f>0.7*D16</f>
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="I17" s="8">
         <v>14.0</v>
       </c>
-      <c r="J17" s="8"/>
+      <c r="J17" s="8">
+        <v>15.0</v>
+      </c>
       <c r="K17" s="7"/>
       <c r="L17" s="8"/>
       <c r="M17" s="8">
@@ -790,17 +806,19 @@
       </c>
       <c r="H18" s="8">
         <f>0.67*D16</f>
-        <v>40.2</v>
+        <v>53.6</v>
       </c>
       <c r="I18" s="8">
         <v>11.0</v>
       </c>
-      <c r="J18" s="8"/>
+      <c r="J18" s="8">
+        <v>10.0</v>
+      </c>
       <c r="K18" s="7"/>
       <c r="L18" s="8"/>
       <c r="M18" s="8">
         <f>IF(D16=0, 0, H18/D16)*H23 + IF(D20=0, 0, I18/D20)*I23 + IF(D21=0, 0, J18/D21)*J23 + IF(D22=0, 0, K18/D22)*K23 + IF(D23=0, 0, L18/D23)*L23</f>
-        <v>28.53571429</v>
+        <v>27.64285714</v>
       </c>
     </row>
     <row r="19">
@@ -821,17 +839,19 @@
       </c>
       <c r="H19" s="8">
         <f>0.63*D16</f>
-        <v>37.8</v>
+        <v>50.4</v>
       </c>
       <c r="I19" s="8">
         <v>8.0</v>
       </c>
-      <c r="J19" s="8"/>
+      <c r="J19" s="8">
+        <v>7.0</v>
+      </c>
       <c r="K19" s="7"/>
       <c r="L19" s="8"/>
       <c r="M19" s="8">
         <f>IF(D16=0, 0, H19/D16)*H23 + IF(D20=0, 0, I19/D20)*I23 + IF(D21=0, 0, J19/D21)*J23 + IF(D22=0, 0, K19/D22)*K23 + IF(D23=0, 0, L19/D23)*L23</f>
-        <v>24.32142857</v>
+        <v>23.53571429</v>
       </c>
     </row>
     <row r="20">
@@ -850,17 +870,19 @@
       </c>
       <c r="H20" s="8">
         <f>0.6*D16</f>
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="I20" s="8">
         <v>4.0</v>
       </c>
-      <c r="J20" s="8"/>
+      <c r="J20" s="8">
+        <v>4.0</v>
+      </c>
       <c r="K20" s="7"/>
       <c r="L20" s="8"/>
       <c r="M20" s="8">
         <f>IF(D16=0, 0, H20/D16)*H23 + IF(D20=0, 0, I20/D20)*I23 + IF(D21=0, 0, J20/D21)*J23 + IF(D22=0, 0, K20/D22)*K23 + IF(D23=0, 0, L20/D23)*L23</f>
-        <v>19.28571429</v>
+        <v>19.14285714</v>
       </c>
     </row>
     <row r="21">
@@ -868,8 +890,11 @@
         <v>18</v>
       </c>
       <c r="C21" s="6"/>
+      <c r="D21" s="3">
+        <v>75.0</v>
+      </c>
       <c r="E21" s="3">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>41</v>
@@ -881,7 +906,9 @@
       <c r="I21" s="8">
         <v>0.0</v>
       </c>
-      <c r="J21" s="8"/>
+      <c r="J21" s="8">
+        <v>0.0</v>
+      </c>
       <c r="K21" s="7"/>
       <c r="L21" s="8"/>
       <c r="M21" s="8">
@@ -941,11 +968,11 @@
       </c>
       <c r="I23" s="8">
         <f>75*E20/(E20+E21+E22+2*E23)</f>
-        <v>75</v>
+        <v>37.5</v>
       </c>
       <c r="J23" s="8">
         <f>75*E21/(E20+E21+E22+2*E23)</f>
-        <v>0</v>
+        <v>37.5</v>
       </c>
       <c r="K23" s="8">
         <f>75*E22/(E20+E21+E22+2*E23)</f>

</xml_diff>

<commit_message>
posted final exam gradelines
</commit_message>
<xml_diff>
--- a/418_S25/gradelines.xlsx
+++ b/418_S25/gradelines.xlsx
@@ -460,7 +460,7 @@
       </c>
       <c r="D2" s="2">
         <f>100*(SUM(E6:E15)/COUNT(E6:E15)*0.25 + SUM(E20:E22)*0.15 + E23*0.3)</f>
-        <v>67.5</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -585,10 +585,12 @@
       <c r="K10" s="7">
         <v>61.0</v>
       </c>
-      <c r="L10" s="8"/>
+      <c r="L10" s="8">
+        <v>87.0</v>
+      </c>
       <c r="M10" s="8">
         <f>IF(D16=0, 0, H10/D16)*H23 + IF(D20=0, 0, I10/D20)*I23 + IF(D21=0, 0, J10/D21)*J23 + IF(D22=0, 0, K10/D22)*K23 + IF(D23=0, 0, L10/D23)*L23</f>
-        <v>85.03571429</v>
+        <v>83.625</v>
       </c>
     </row>
     <row r="11">
@@ -618,10 +620,12 @@
       <c r="K11" s="7">
         <v>54.0</v>
       </c>
-      <c r="L11" s="8"/>
+      <c r="L11" s="8">
+        <v>75.0</v>
+      </c>
       <c r="M11" s="8">
         <f>IF(D16=0, 0, H11/D16)*H23 + IF(D20=0, 0, I11/D20)*I23 + IF(D21=0, 0, J11/D21)*J23 + IF(D22=0, 0, K11/D22)*K23 + IF(D23=0, 0, L11/D23)*L23</f>
-        <v>77.30952381</v>
+        <v>75.475</v>
       </c>
     </row>
     <row r="12">
@@ -651,10 +655,12 @@
       <c r="K12" s="7">
         <v>47.0</v>
       </c>
-      <c r="L12" s="8"/>
+      <c r="L12" s="8">
+        <v>64.0</v>
+      </c>
       <c r="M12" s="8">
         <f>IF(D16=0, 0, H12/D16)*H23 + IF(D20=0, 0, I12/D20)*I23 + IF(D21=0, 0, J12/D21)*J23 + IF(D22=0, 0, K12/D22)*K23 + IF(D23=0, 0, L12/D23)*L23</f>
-        <v>69.58333333</v>
+        <v>67.59285714</v>
       </c>
     </row>
     <row r="13">
@@ -684,10 +690,12 @@
       <c r="K13" s="7">
         <v>40.0</v>
       </c>
-      <c r="L13" s="8"/>
+      <c r="L13" s="8">
+        <v>53.0</v>
+      </c>
       <c r="M13" s="8">
         <f>IF(D16=0, 0, H13/D16)*H23 + IF(D20=0, 0, I13/D20)*I23 + IF(D21=0, 0, J13/D21)*J23 + IF(D22=0, 0, K13/D22)*K23 + IF(D23=0, 0, L13/D23)*L23</f>
-        <v>61.60714286</v>
+        <v>59.46071429</v>
       </c>
     </row>
     <row r="14">
@@ -717,10 +725,12 @@
       <c r="K14" s="7">
         <v>33.0</v>
       </c>
-      <c r="L14" s="8"/>
+      <c r="L14" s="8">
+        <v>42.0</v>
+      </c>
       <c r="M14" s="8">
         <f>IF(D16=0, 0, H14/D16)*H23 + IF(D20=0, 0, I14/D20)*I23 + IF(D21=0, 0, J14/D21)*J23 + IF(D22=0, 0, K14/D22)*K23 + IF(D23=0, 0, L14/D23)*L23</f>
-        <v>53.88095238</v>
+        <v>51.57857143</v>
       </c>
     </row>
     <row r="15">
@@ -732,7 +742,7 @@
         <v>20.0</v>
       </c>
       <c r="E15" s="7">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>33</v>
@@ -750,10 +760,12 @@
       <c r="K15" s="7">
         <v>26.0</v>
       </c>
-      <c r="L15" s="8"/>
+      <c r="L15" s="8">
+        <v>30.0</v>
+      </c>
       <c r="M15" s="8">
         <f>IF(D16=0, 0, H15/D16)*H23 + IF(D20=0, 0, I15/D20)*I23 + IF(D21=0, 0, J15/D21)*J23 + IF(D22=0, 0, K15/D22)*K23 + IF(D23=0, 0, L15/D23)*L23</f>
-        <v>46.1547619</v>
+        <v>43.42857143</v>
       </c>
     </row>
     <row r="16">
@@ -787,10 +799,12 @@
       <c r="K16" s="7">
         <v>20.0</v>
       </c>
-      <c r="L16" s="8"/>
+      <c r="L16" s="8">
+        <v>25.0</v>
+      </c>
       <c r="M16" s="8">
         <f>IF(D16=0, 0, H16/D16)*H23 + IF(D20=0, 0, I16/D20)*I23 + IF(D21=0, 0, J16/D21)*J23 + IF(D22=0, 0, K16/D22)*K23 + IF(D23=0, 0, L16/D23)*L23</f>
-        <v>39.20238095</v>
+        <v>37.51785714</v>
       </c>
     </row>
     <row r="17">
@@ -810,10 +824,12 @@
       <c r="K17" s="7">
         <v>14.0</v>
       </c>
-      <c r="L17" s="8"/>
+      <c r="L17" s="8">
+        <v>20.0</v>
+      </c>
       <c r="M17" s="8">
         <f>IF(D16=0, 0, H17/D16)*H23 + IF(D20=0, 0, I17/D20)*I23 + IF(D21=0, 0, J17/D21)*J23 + IF(D22=0, 0, K17/D22)*K23 + IF(D23=0, 0, L17/D23)*L23</f>
-        <v>32.5</v>
+        <v>31.85714286</v>
       </c>
     </row>
     <row r="18">
@@ -833,10 +849,12 @@
       <c r="K18" s="7">
         <v>11.0</v>
       </c>
-      <c r="L18" s="8"/>
+      <c r="L18" s="8">
+        <v>15.0</v>
+      </c>
       <c r="M18" s="8">
         <f>IF(D16=0, 0, H18/D16)*H23 + IF(D20=0, 0, I18/D20)*I23 + IF(D21=0, 0, J18/D21)*J23 + IF(D22=0, 0, K18/D22)*K23 + IF(D23=0, 0, L18/D23)*L23</f>
-        <v>27.94047619</v>
+        <v>27.48214286</v>
       </c>
     </row>
     <row r="19">
@@ -868,10 +886,12 @@
       <c r="K19" s="7">
         <v>8.0</v>
       </c>
-      <c r="L19" s="8"/>
+      <c r="L19" s="8">
+        <v>10.0</v>
+      </c>
       <c r="M19" s="8">
         <f>IF(D16=0, 0, H19/D16)*H23 + IF(D20=0, 0, I19/D20)*I23 + IF(D21=0, 0, J19/D21)*J23 + IF(D22=0, 0, K19/D22)*K23 + IF(D23=0, 0, L19/D23)*L23</f>
-        <v>23.79761905</v>
+        <v>23.25714286</v>
       </c>
     </row>
     <row r="20">
@@ -901,10 +921,12 @@
       <c r="K20" s="7">
         <v>4.0</v>
       </c>
-      <c r="L20" s="8"/>
+      <c r="L20" s="8">
+        <v>5.0</v>
+      </c>
       <c r="M20" s="8">
         <f>IF(D16=0, 0, H20/D16)*H23 + IF(D20=0, 0, I20/D20)*I23 + IF(D21=0, 0, J20/D21)*J23 + IF(D22=0, 0, K20/D22)*K23 + IF(D23=0, 0, L20/D23)*L23</f>
-        <v>19.19047619</v>
+        <v>18.85357143</v>
       </c>
     </row>
     <row r="21">
@@ -934,7 +956,9 @@
       <c r="K21" s="7">
         <v>0.0</v>
       </c>
-      <c r="L21" s="8"/>
+      <c r="L21" s="8">
+        <v>0.0</v>
+      </c>
       <c r="M21" s="8">
         <f>IF(D16=0, 0, H21/D16)*H23 + IF(D20=0, 0, I21/D20)*I23 + IF(D21=0, 0, J21/D21)*J23 + IF(D22=0, 0, K21/D22)*K23 + IF(D23=0, 0, L21/D23)*L23</f>
         <v>0</v>
@@ -984,8 +1008,11 @@
         <v>20</v>
       </c>
       <c r="C23" s="6"/>
+      <c r="D23" s="3">
+        <v>112.0</v>
+      </c>
       <c r="E23" s="3">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>42</v>
@@ -995,19 +1022,19 @@
       </c>
       <c r="I23" s="8">
         <f>75*E20/(E20+E21+E22+2*E23)</f>
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="J23" s="8">
         <f>75*E21/(E20+E21+E22+2*E23)</f>
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="K23" s="8">
         <f>75*E22/(E20+E21+E22+2*E23)</f>
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="L23" s="8">
         <f>75*2*E23/(E20+E21+E22+2*E23)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="M23" s="8">
         <f>SUM(H23:L23)</f>

</xml_diff>